<commit_message>
Multiple longest words tests
</commit_message>
<xml_diff>
--- a/doc/Sentences_TestSuite_0.1.xlsx
+++ b/doc/Sentences_TestSuite_0.1.xlsx
@@ -21,14 +21,17 @@
     <sheet name="3.1.0 Numbers" sheetId="7" r:id="rId7"/>
     <sheet name="4.1.0 Commas ellipses" sheetId="8" r:id="rId8"/>
     <sheet name="4.2.0 Periods" sheetId="9" r:id="rId9"/>
-    <sheet name="5.1.0 Spaces" sheetId="10" r:id="rId10"/>
-    <sheet name="6.1.0 Accents" sheetId="11" r:id="rId11"/>
-    <sheet name="6.2.0 Apostrophes" sheetId="12" r:id="rId12"/>
-    <sheet name="6.3.0 Foreign characters" sheetId="13" r:id="rId13"/>
-    <sheet name="6.4.0 Other characers" sheetId="14" r:id="rId14"/>
-    <sheet name="6.5.0 Quotes" sheetId="15" r:id="rId15"/>
-    <sheet name="6.6.0 Single dashes" sheetId="16" r:id="rId16"/>
-    <sheet name="7.1.0 Case-Sentitivity" sheetId="17" r:id="rId17"/>
+    <sheet name="5.1.0 Multiple sentence" sheetId="10" r:id="rId10"/>
+    <sheet name="5.2.0 No sentence punctuation" sheetId="11" r:id="rId11"/>
+    <sheet name="5.3.0 Single sentence" sheetId="12" r:id="rId12"/>
+    <sheet name="6.1.0 Spaces" sheetId="13" r:id="rId13"/>
+    <sheet name="7.1.0 Accents" sheetId="14" r:id="rId14"/>
+    <sheet name="7.2.0 Apostrophes" sheetId="15" r:id="rId15"/>
+    <sheet name="7.3.0 Foreign characters" sheetId="16" r:id="rId16"/>
+    <sheet name="7.4.0 Other characers" sheetId="17" r:id="rId17"/>
+    <sheet name="7.5.0 Quotes" sheetId="18" r:id="rId18"/>
+    <sheet name="7.6.0 Single dashes" sheetId="19" r:id="rId19"/>
+    <sheet name="8.1.0 Case-Sentitivity" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -151,6 +154,23 @@
     <t>Multiple longest words</t>
   </si>
   <si>
+    <t xml:space="preserve">Verify multiple longest words are returned when they are the same length.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found even when there is more than one. Each longest word should be returned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					I can ride a bike.
+					Do not tie your shoes today.
+					Clean your room or I will get very angry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	5, ride bike
+	6, shoes today
+	9, Clean angry</t>
+  </si>
+  <si>
     <t>2.3.1.1</t>
   </si>
   <si>
@@ -167,6 +187,82 @@
   </si>
   <si>
     <t>Commas ellipses</t>
+  </si>
+  <si>
+    <t>Commas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify words are matched even when they are followed by commas.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found when it is followed by a comma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					I had cake, milk, soda, and tea.
+					I had cake.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	7, cake milk soda
+	3, cake</t>
+  </si>
+  <si>
+    <t>4.1.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify words are matched when followed by commas but the commas are not matched.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found when it is followed by a comma but the comma should not be matched.</t>
+  </si>
+  <si>
+    <t>4.1.2.1</t>
+  </si>
+  <si>
+    <t>Ellipses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify words are matched even when they are followed by ellipses.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found when it is followed by ellipses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					We visited the lake... and came back the next day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	10, visited</t>
+  </si>
+  <si>
+    <t>4.1.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify words are matched even when they are preceded by ellipses.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found when it is preceded by ellipses. A sentence should not be considered ended by the period in an ellipses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					We visited the lake... and came back to Washington DC the next day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	13, Washington</t>
+  </si>
+  <si>
+    <t>4.1.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify words are matched when followed by ellipses but the ellipses are not matched.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					We visited lake Michigan... and came back the next day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	10, Michigan</t>
   </si>
   <si>
     <t>4.2.1.1</t>
@@ -191,6 +287,75 @@
     <t>5.1.1.1</t>
   </si>
   <si>
+    <t>Multiple sentence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot parse words when more than one sentence is provided.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should not be found when more than one sentence is provided. An exception should be thrown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">				1. Provide the sentences as an input.
+				2. Examine the word count and longest word returned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					I woke up. I went for a jog.
+					I woke up! I went for a jog!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">			Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	An exception is thrown.</t>
+  </si>
+  <si>
+    <t>5.2.1.1</t>
+  </si>
+  <si>
+    <t>No sentence punctuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the proper word count and longest word is returned even when no sentence punctuation is present.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found, along with the word count, even when sentence punctuation is ommited. Matches should occur regardless of whether a final punctuation mark is present and regardless of whether any other punctuation is present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					We tried to swim near the lake
+					We tried to swim near the lake and found a snake
+					We tried to swim near the lake We went home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	7, tried
+	11, tried found snake
+	10, tried</t>
+  </si>
+  <si>
+    <t>5.3.1.1</t>
+  </si>
+  <si>
+    <t>Single sentence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the proper word count and longest word is returned for a single sentence.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		The longest word in a sentence should be found, along with the word count, when a single sentence is provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					We tried to swim near the lake.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	7, tried</t>
+  </si>
+  <si>
+    <t>6.1.1.1</t>
+  </si>
+  <si>
     <t>Spaces</t>
   </si>
   <si>
@@ -209,49 +374,49 @@
 	8, alligator</t>
   </si>
   <si>
-    <t>6.1.1.1</t>
+    <t>7.1.1.1</t>
   </si>
   <si>
     <t>Accents</t>
   </si>
   <si>
-    <t>6.2.1.1</t>
+    <t>7.2.1.1</t>
   </si>
   <si>
     <t>Apostrophes</t>
   </si>
   <si>
-    <t>6.3.1.1</t>
+    <t>7.3.1.1</t>
   </si>
   <si>
     <t>Foreign characters</t>
   </si>
   <si>
-    <t>6.4.1.1</t>
+    <t>7.4.1.1</t>
   </si>
   <si>
     <t>Other characers</t>
   </si>
   <si>
-    <t>6.5.1.1</t>
+    <t>7.5.1.1</t>
   </si>
   <si>
     <t>Quotes</t>
   </si>
   <si>
-    <t>6.6.1.1</t>
+    <t>7.6.1.1</t>
   </si>
   <si>
     <t>Single dashes</t>
   </si>
   <si>
-    <t>7.1.1.1</t>
+    <t>8.1.1.1</t>
   </si>
   <si>
     <t>Case-Sentitivity</t>
   </si>
   <si>
-    <t>7.1.1.2</t>
+    <t>8.1.1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Verify words in capital letters only are matched.
@@ -686,7 +851,7 @@
   <dimension ref="B1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -942,37 +1107,37 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="2:24" ht="72" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="48" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1090,37 +1255,37 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="96" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1238,37 +1403,37 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="36" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1386,37 +1551,37 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="72" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1536,10 +1701,10 @@
     </row>
     <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>20</v>
@@ -1684,10 +1849,10 @@
     </row>
     <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>20</v>
@@ -1832,10 +1997,10 @@
     </row>
     <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>20</v>
@@ -1870,7 +2035,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X4"/>
+  <dimension ref="B1:X3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
@@ -1980,10 +2145,10 @@
     </row>
     <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>20</v>
@@ -2011,37 +2176,300 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:24" ht="48" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="16" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:X3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="4" width="14.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="4.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="37.08984375" customWidth="1"/>
+    <col min="7" max="7" width="36.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="1.36328125" customWidth="1"/>
+    <col min="10" max="10" width="31.6328125" customWidth="1"/>
+    <col min="11" max="11" width="1.36328125" customWidth="1"/>
+    <col min="12" max="12" width="5.90625" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" customWidth="1"/>
+    <col min="15" max="15" width="1.36328125" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" customWidth="1"/>
+    <col min="17" max="17" width="64.6328125" customWidth="1"/>
+    <col min="18" max="18" width="10.36328125" customWidth="1"/>
+    <col min="19" max="19" width="1.36328125" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="9" customWidth="1"/>
+    <col min="21" max="21" width="34.08984375" style="10" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="12"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+      <c r="B3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="P3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:X3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="4" width="14.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="4.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="37.08984375" customWidth="1"/>
+    <col min="7" max="7" width="36.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="1.36328125" customWidth="1"/>
+    <col min="10" max="10" width="31.6328125" customWidth="1"/>
+    <col min="11" max="11" width="1.36328125" customWidth="1"/>
+    <col min="12" max="12" width="5.90625" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" customWidth="1"/>
+    <col min="15" max="15" width="1.36328125" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" customWidth="1"/>
+    <col min="17" max="17" width="64.6328125" customWidth="1"/>
+    <col min="18" max="18" width="10.36328125" customWidth="1"/>
+    <col min="19" max="19" width="1.36328125" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="9" customWidth="1"/>
+    <col min="21" max="21" width="34.08984375" style="10" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="18" t="s">
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="12"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+      <c r="B3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="18"/>
-      <c r="P4" s="18" t="s">
+      <c r="M3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="18" t="s">
-        <v>71</v>
+      <c r="Q3" s="18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2197,6 +2625,187 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:X4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="4" width="14.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="4.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="37.08984375" customWidth="1"/>
+    <col min="7" max="7" width="36.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="1.36328125" customWidth="1"/>
+    <col min="10" max="10" width="31.6328125" customWidth="1"/>
+    <col min="11" max="11" width="1.36328125" customWidth="1"/>
+    <col min="12" max="12" width="5.90625" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" customWidth="1"/>
+    <col min="15" max="15" width="1.36328125" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" customWidth="1"/>
+    <col min="17" max="17" width="64.6328125" customWidth="1"/>
+    <col min="18" max="18" width="10.36328125" customWidth="1"/>
+    <col min="19" max="19" width="1.36328125" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="9" customWidth="1"/>
+    <col min="21" max="21" width="34.08984375" style="10" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="12"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+      <c r="B3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="P3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="48" x14ac:dyDescent="0.35">
+      <c r="B4" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="17">
+        <v>2</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="18"/>
+      <c r="P4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X3"/>
@@ -2603,7 +3212,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="84" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>33</v>
       </c>
@@ -2611,29 +3220,29 @@
         <v>34</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2753,10 +3362,10 @@
     </row>
     <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>20</v>
@@ -2901,10 +3510,10 @@
     </row>
     <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>20</v>
@@ -2939,7 +3548,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X3"/>
+  <dimension ref="B1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
@@ -3047,37 +3656,169 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="2:24" ht="60" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="36" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>26</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="36" x14ac:dyDescent="0.35">
+      <c r="B4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="17">
+        <v>2</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="18"/>
+      <c r="P4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" ht="36" x14ac:dyDescent="0.35">
+      <c r="B5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="17">
+        <v>3</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="18"/>
+      <c r="P5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" ht="48" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="17">
+        <v>4</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="18"/>
+      <c r="P6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" ht="36" x14ac:dyDescent="0.35">
+      <c r="B7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="17">
+        <v>5</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="18"/>
+      <c r="P7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3197,35 +3938,35 @@
     </row>
     <row r="3" spans="2:24" ht="36" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="N3" s="18"/>
       <c r="P3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>